<commit_message>
completed transition to GAMS wrappers for input data
data preprocessing and instantiation now works with GAMS wrappers, which is faster and easier to maintain.
</commit_message>
<xml_diff>
--- a/data/processed/plant_props.xlsx
+++ b/data/processed/plant_props.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186022E7-AFC8-4C89-8CBD-B7B370B26677}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD4BC5-0E4B-414F-8951-A6EF5FD4227B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="8520" windowWidth="21600" windowHeight="6390" firstSheet="4" activeTab="13" xr2:uid="{2420223F-F471-4634-842A-824E9D1ECD47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="10" xr2:uid="{2420223F-F471-4634-842A-824E9D1ECD47}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity" sheetId="5" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="165">
   <si>
     <t>Nuclear</t>
   </si>
@@ -834,15 +834,6 @@
   </si>
   <si>
     <t>om_fix</t>
-  </si>
-  <si>
-    <t>power_prp</t>
-  </si>
-  <si>
-    <t>heat_prp</t>
-  </si>
-  <si>
-    <t>fuel_prp</t>
   </si>
   <si>
     <t>1) Multiply power and heat by MW</t>
@@ -4860,7 +4851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4875,13 +4868,13 @@
         <v>85</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -8051,7 +8044,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1">
         <v>0.03</v>
@@ -8074,18 +8067,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B2">
         <v>25</v>
@@ -8100,7 +8093,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -8115,7 +8108,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -8130,7 +8123,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B5">
         <v>25</v>
@@ -8152,7 +8145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P26" sqref="P26"/>
     </sheetView>
@@ -8167,7 +8160,7 @@
         <v>101</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>47</v>
@@ -8206,13 +8199,13 @@
         <v>103</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -8220,7 +8213,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>24</v>
@@ -8274,7 +8267,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -8328,7 +8321,7 @@
         <v>20.5</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -8382,7 +8375,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -8436,7 +8429,7 @@
         <v>21.5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -8490,7 +8483,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -8544,7 +8537,7 @@
         <v>30.5</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -8598,7 +8591,7 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -8652,7 +8645,7 @@
         <v>31.5</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -8706,7 +8699,7 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -8760,7 +8753,7 @@
         <v>32.5</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -8814,7 +8807,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -8868,7 +8861,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -8922,7 +8915,7 @@
         <v>40.5</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -8976,7 +8969,7 @@
         <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -9030,7 +9023,7 @@
         <v>41.5</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -9084,7 +9077,7 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -9138,7 +9131,7 @@
         <v>42.5</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -9192,7 +9185,7 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -9246,7 +9239,7 @@
         <v>43.5</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -9300,7 +9293,7 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -9354,7 +9347,7 @@
         <v>44.5</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -9408,7 +9401,7 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -9462,7 +9455,7 @@
         <v>45.5</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -9516,7 +9509,7 @@
         <v>49.5</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -9570,7 +9563,7 @@
         <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -9624,7 +9617,7 @@
         <v>50.5</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -9678,7 +9671,7 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -9732,7 +9725,7 @@
         <v>51.5</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -9786,7 +9779,7 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -9840,7 +9833,7 @@
         <v>52.5</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -9894,7 +9887,7 @@
         <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -9948,7 +9941,7 @@
         <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -10002,7 +9995,7 @@
         <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -10056,7 +10049,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -10110,7 +10103,7 @@
         <v>70.5</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -10177,57 +10170,57 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
         <v>146</v>
       </c>
-      <c r="C2" t="s">
-        <v>149</v>
-      </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" t="s">
         <v>146</v>
       </c>
-      <c r="G2" t="s">
-        <v>149</v>
-      </c>
       <c r="H2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -10439,48 +10432,48 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
         <v>150</v>
       </c>
-      <c r="C1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1" t="s">
         <v>157</v>
-      </c>
-      <c r="F1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M1" t="s">
-        <v>156</v>
-      </c>
-      <c r="N1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2">
         <v>1200</v>
@@ -10503,7 +10496,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H3">
         <v>600</v>
@@ -10514,7 +10507,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B4">
         <v>1200</v>
@@ -10525,7 +10518,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>700</v>
@@ -10542,7 +10535,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <v>4500</v>
@@ -10562,7 +10555,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F7">
         <v>800</v>
@@ -10570,7 +10563,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C8">
         <v>600</v>
@@ -10587,7 +10580,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B9">
         <v>300</v>
@@ -10595,7 +10588,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -10606,7 +10599,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C11">
         <v>950</v>
@@ -10614,7 +10607,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E12">
         <v>600</v>
@@ -10625,7 +10618,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B13">
         <v>950</v>
@@ -10633,7 +10626,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E14">
         <v>800</v>
@@ -15390,7 +15383,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -15407,7 +15400,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
building up capacities for policy paper
</commit_message>
<xml_diff>
--- a/data/processed/plant_props.xlsx
+++ b/data/processed/plant_props.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D0591C-6F72-4C51-AC9C-15FB336CF5CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB375526-7B2B-47EE-8CCB-15F1FE6F78D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{2420223F-F471-4634-842A-824E9D1ECD47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="11" xr2:uid="{2420223F-F471-4634-842A-824E9D1ECD47}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity" sheetId="5" r:id="rId1"/>
@@ -2428,7 +2428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7768,7 +7768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -10977,7 +10977,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11001,11 +11001,11 @@
         <v>25</v>
       </c>
       <c r="C2" s="20">
-        <v>900000</v>
+        <v>692940</v>
       </c>
       <c r="D2" s="20">
         <f>C2*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>51685.083935215036</v>
+        <v>39794.068957853233</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11063,8 +11063,8 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P26" sqref="P26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12522,11 +12522,11 @@
         <v>35</v>
       </c>
       <c r="P27" s="20">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="Q27" s="20">
         <f>P27*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>17304.951156185158</v>
+        <v>21631.18894523145</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -12576,11 +12576,11 @@
         <v>35</v>
       </c>
       <c r="P28" s="20">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="Q28" s="20">
         <f>P28*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>17304.951156185158</v>
+        <v>21631.18894523145</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -12630,11 +12630,11 @@
         <v>35</v>
       </c>
       <c r="P29" s="20">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="Q29" s="20">
         <f>P29*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>17304.951156185158</v>
+        <v>21631.18894523145</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -12684,11 +12684,11 @@
         <v>35</v>
       </c>
       <c r="P30" s="20">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="Q30" s="20">
         <f>P30*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>17304.951156185158</v>
+        <v>21631.18894523145</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -12738,11 +12738,11 @@
         <v>35</v>
       </c>
       <c r="P31" s="20">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="Q31" s="20">
         <f>P31*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>17304.951156185158</v>
+        <v>21631.18894523145</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -12792,11 +12792,11 @@
         <v>35</v>
       </c>
       <c r="P32" s="20">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="Q32" s="20">
         <f>P32*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>17304.951156185158</v>
+        <v>21631.18894523145</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -13558,7 +13558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B592C-F134-4F63-8551-B8C145671911}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated cost of intermittens power generators
set all investment cost proportional to full load hours so that each technology has same lcoe
</commit_message>
<xml_diff>
--- a/data/processed/plant_props.xlsx
+++ b/data/processed/plant_props.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB375526-7B2B-47EE-8CCB-15F1FE6F78D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="11" xr2:uid="{2420223F-F471-4634-842A-824E9D1ECD47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity" sheetId="5" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <sheet name="itm_invest" sheetId="19" r:id="rId14"/>
     <sheet name="flex_params" sheetId="17" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="J7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -186,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="J9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="J11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+    <comment ref="J13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
+    <comment ref="J16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
+    <comment ref="J18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -306,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
+    <comment ref="J20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
+    <comment ref="J22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
+    <comment ref="J26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -378,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
+    <comment ref="J29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
+    <comment ref="J31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
+    <comment ref="B37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -455,12 +454,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="B37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -489,12 +488,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="B37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -523,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="169">
   <si>
     <t>Nuclear</t>
   </si>
@@ -1019,11 +1018,23 @@
   <si>
     <t>ng_boiler_chp</t>
   </si>
+  <si>
+    <t>invest-AT</t>
+  </si>
+  <si>
+    <t>annuity-AT</t>
+  </si>
+  <si>
+    <t>invest-DE</t>
+  </si>
+  <si>
+    <t>annuity-DE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1196,7 +1207,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1315,7 +1326,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4946-A54F-ABD3-318F1D455BE1}"/>
             </c:ext>
@@ -1329,11 +1340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="557806680"/>
-        <c:axId val="191249208"/>
+        <c:axId val="528318328"/>
+        <c:axId val="528319112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="557806680"/>
+        <c:axId val="528318328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1390,12 +1401,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191249208"/>
+        <c:crossAx val="528319112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191249208"/>
+        <c:axId val="528319112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,7 +1463,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="557806680"/>
+        <c:crossAx val="528318328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1466,14 +1477,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2084,7 +2095,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A8A110-A4AD-3D40-8A68-7F329A42582D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09A8A110-A4AD-3D40-8A68-7F329A42582D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2106,7 +2117,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2181,23 +2192,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2233,23 +2227,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2425,7 +2402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0"/>
@@ -4527,7 +4504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T149"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7443,7 +7420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7765,10 +7742,10 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -10950,7 +10927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7C8975-A305-4E1C-AF87-2937CECBD9B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10973,27 +10950,33 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7EBE7A-C293-4DB8-B9CD-A8BF486AE839}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -11004,11 +10987,18 @@
         <v>692940</v>
       </c>
       <c r="D2" s="20">
+        <v>624424.76</v>
+      </c>
+      <c r="E2" s="20">
         <f>C2*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
         <v>39794.068957853233</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="20">
+        <f>D2*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
+        <v>35859.384590918336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -11016,14 +11006,21 @@
         <v>50</v>
       </c>
       <c r="C3" s="20">
-        <v>3400000</v>
+        <v>3363931.406</v>
       </c>
       <c r="D3" s="20">
+        <v>2378811.3020000001</v>
+      </c>
+      <c r="E3" s="20">
         <f>C3*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>195254.76153303459</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193183.41896823992</v>
+      </c>
+      <c r="F3" s="20">
+        <f>D3*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
+        <v>136610.06867767574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>144</v>
       </c>
@@ -11031,14 +11028,21 @@
         <v>25</v>
       </c>
       <c r="C4" s="20">
-        <v>1750000</v>
+        <v>1749998.46</v>
       </c>
       <c r="D4" s="20">
+        <v>1270661.2620000001</v>
+      </c>
+      <c r="E4" s="20">
         <f>C4*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>100498.77431847369</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100498.68587955227</v>
+      </c>
+      <c r="F4" s="20">
+        <f>D4*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
+        <v>72971.371088551401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -11049,8 +11053,15 @@
         <v>3900000</v>
       </c>
       <c r="D5" s="20">
+        <v>2681281.486</v>
+      </c>
+      <c r="E5" s="20">
         <f>C5*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
         <v>223968.69705259849</v>
+      </c>
+      <c r="F5" s="20">
+        <f>D5*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
+        <v>153980.287397609</v>
       </c>
     </row>
   </sheetData>
@@ -11059,7 +11070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13076,7 +13087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF80946E-D584-4D72-9204-A1B358F8318D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13338,7 +13349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D252CA42-99FF-432E-BE03-B101DB5FA373}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13555,7 +13566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B592C-F134-4F63-8551-B8C145671911}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13706,7 +13717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15579,7 +15590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15875,7 +15886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17011,7 +17022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17962,7 +17973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added wind versus pv analysis
adjusted gms model, incorporated iterations over CO2 prices, added heat pumps to technologies
</commit_message>
<xml_diff>
--- a/data/processed/plant_props.xlsx
+++ b/data/processed/plant_props.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E208F9-1E78-45CA-922E-0232580B2766}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity" sheetId="5" r:id="rId1"/>
@@ -21,9 +22,10 @@
     <sheet name="gen_possibilities" sheetId="16" r:id="rId12"/>
     <sheet name="WACC" sheetId="21" r:id="rId13"/>
     <sheet name="itm_invest" sheetId="19" r:id="rId14"/>
-    <sheet name="flex_params" sheetId="17" r:id="rId15"/>
+    <sheet name="itm_invest_bup" sheetId="23" r:id="rId15"/>
+    <sheet name="flex_params" sheetId="17" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,12 +38,70 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{16E04DA7-1C06-4CAD-8EB0-D57A594E3CCF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Biermayr Innovative Energietechnologien</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D45358AA-A224-4C8D-AEBA-C4FCE55F8E45}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+IG Windkraft</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0" shapeId="0">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -209,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0" shapeId="0">
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
       <text>
         <r>
           <rPr>
@@ -257,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -281,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="0" shapeId="0">
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -305,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0" shapeId="0">
+    <comment ref="J20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -329,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -353,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J26" authorId="0" shapeId="0">
+    <comment ref="J26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -377,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J29" authorId="0" shapeId="0">
+    <comment ref="J29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -401,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J31" authorId="0" shapeId="0">
+    <comment ref="J31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000010000000}">
       <text>
         <r>
           <rPr>
@@ -425,41 +485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Kennlinie von Fraunhofer UMSICHT, basierend auf einem Einspeicherwirkungsgrad von 0,9</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="B37" authorId="0" shapeId="0">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000011000000}">
       <text>
         <r>
           <rPr>
@@ -488,12 +514,46 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B37" authorId="0" shapeId="0">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kennlinie von Fraunhofer UMSICHT, basierend auf einem Einspeicherwirkungsgrad von 0,9</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -522,7 +582,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="171">
   <si>
     <t>Nuclear</t>
   </si>
@@ -1030,16 +1090,24 @@
   <si>
     <t>annuity-DE</t>
   </si>
+  <si>
+    <t>Power - Heatpump</t>
+  </si>
+  <si>
+    <t>heatpump_pth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1095,6 +1163,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1159,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1189,6 +1270,9 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1207,7 +1291,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1326,7 +1410,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4946-A54F-ABD3-318F1D455BE1}"/>
             </c:ext>
@@ -1477,14 +1561,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2095,7 +2179,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09A8A110-A4AD-3D40-8A68-7F329A42582D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A8A110-A4AD-3D40-8A68-7F329A42582D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2117,7 +2201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2192,6 +2276,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2227,6 +2328,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2402,10 +2520,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4504,7 +4622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T149"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7420,10 +7538,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7735,6 +7855,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>100</v>
+      </c>
+      <c r="B39" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7742,11 +7870,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H186"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="A192" sqref="A192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10751,7 +10879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="16">
         <v>70</v>
       </c>
@@ -10768,7 +10896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="16">
         <v>70</v>
       </c>
@@ -10785,7 +10913,7 @@
         <v>0.85419999999999996</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="16">
         <v>70</v>
       </c>
@@ -10802,7 +10930,7 @@
         <v>0.54049999999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="16">
         <v>70</v>
       </c>
@@ -10819,7 +10947,7 @@
         <v>0.65790000000000004</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="16">
         <v>70</v>
       </c>
@@ -10836,7 +10964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="16">
         <v>70.5</v>
       </c>
@@ -10853,7 +10981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="16">
         <v>70.5</v>
       </c>
@@ -10870,7 +10998,7 @@
         <v>0.85419999999999996</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="16">
         <v>70.5</v>
       </c>
@@ -10887,7 +11015,7 @@
         <v>0.54049999999999998</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="16">
         <v>70.5</v>
       </c>
@@ -10904,7 +11032,7 @@
         <v>0.65790000000000004</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="16">
         <v>70.5</v>
       </c>
@@ -10918,6 +11046,97 @@
         <v>0</v>
       </c>
       <c r="E186" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="16">
+        <v>100</v>
+      </c>
+      <c r="B187" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C187" s="15">
+        <v>0</v>
+      </c>
+      <c r="D187" s="15">
+        <v>3</v>
+      </c>
+      <c r="E187" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="16">
+        <v>100</v>
+      </c>
+      <c r="B188" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C188" s="15">
+        <v>0</v>
+      </c>
+      <c r="D188" s="15">
+        <f>$D$187*$E188+ROUND(LOG(E188)*0.25,3)</f>
+        <v>2.2189999999999999</v>
+      </c>
+      <c r="E188" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F188" s="15"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="16">
+        <v>100</v>
+      </c>
+      <c r="B189" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189" s="15">
+        <v>0</v>
+      </c>
+      <c r="D189" s="15">
+        <f t="shared" ref="D189:D191" si="0">$D$187*$E189+ROUND(LOG(E189)*0.25,3)</f>
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="E189" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="F189" s="15"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="16">
+        <v>100</v>
+      </c>
+      <c r="B190" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="15">
+        <v>0</v>
+      </c>
+      <c r="D190" s="15">
+        <f t="shared" si="0"/>
+        <v>1.425</v>
+      </c>
+      <c r="E190" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F190" s="15"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="16">
+        <v>100</v>
+      </c>
+      <c r="B191" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C191" s="15">
+        <v>0</v>
+      </c>
+      <c r="D191" s="15">
+        <v>0</v>
+      </c>
+      <c r="E191" s="15">
         <v>0</v>
       </c>
     </row>
@@ -10927,21 +11146,32 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>161</v>
       </c>
-      <c r="B1">
-        <v>0.03</v>
+      <c r="B2">
+        <v>0.05</v>
+      </c>
+      <c r="C2">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -10950,16 +11180,19 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>163</v>
       </c>
@@ -10976,7 +11209,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -10984,43 +11217,47 @@
         <v>25</v>
       </c>
       <c r="C2" s="20">
-        <v>692940</v>
+        <v>560000</v>
       </c>
       <c r="D2" s="20">
-        <v>624424.76</v>
+        <v>560000</v>
       </c>
       <c r="E2" s="20">
-        <f>C2*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>39794.068957853233</v>
+        <f>C2*(WACC!$B$2*(1+WACC!$B$2)^$B2)/((1+WACC!$B$2)^$B2-1)</f>
+        <v>39733.376087568584</v>
       </c>
       <c r="F2" s="20">
-        <f>D2*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>35859.384590918336</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <f>D2*(WACC!$C$2*(1+WACC!$C$2)^$B2)/((1+WACC!$C$2)^$B2-1)</f>
+        <v>35846.699160414559</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C3" s="20">
-        <v>3363931.406</v>
+        <v>3800000</v>
       </c>
       <c r="D3" s="20">
-        <v>2378811.3020000001</v>
+        <v>3800000</v>
       </c>
       <c r="E3" s="20">
-        <f>C3*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>193183.41896823992</v>
+        <f>C3*(WACC!$B$2*(1+WACC!$B$2)^$B3)/((1+WACC!$B$2)^$B3-1)</f>
+        <v>195022.11237084537</v>
       </c>
       <c r="F3" s="20">
-        <f>D3*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>136610.06867767574</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <f>D3*(WACC!$C$2*(1+WACC!$C$2)^$B3)/((1+WACC!$C$2)^$B3-1)</f>
+        <v>160470.20579380851</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>144</v>
       </c>
@@ -11028,21 +11265,23 @@
         <v>25</v>
       </c>
       <c r="C4" s="20">
-        <v>1749998.46</v>
+        <v>1250000</v>
       </c>
       <c r="D4" s="20">
-        <v>1270661.2620000001</v>
+        <v>1200000</v>
       </c>
       <c r="E4" s="20">
-        <f>C4*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>100498.68587955227</v>
+        <f>C4*(WACC!$B$2*(1+WACC!$B$2)^$B4)/((1+WACC!$B$2)^$B4-1)</f>
+        <v>88690.571624037024</v>
       </c>
       <c r="F4" s="20">
-        <f>D4*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>72971.371088551401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <f>D4*(WACC!$C$2*(1+WACC!$C$2)^$B4)/((1+WACC!$C$2)^$B4-1)</f>
+        <v>76814.355343745483</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -11050,19 +11289,59 @@
         <v>25</v>
       </c>
       <c r="C5" s="20">
-        <v>3900000</v>
+        <v>2400000</v>
       </c>
       <c r="D5" s="20">
-        <v>2681281.486</v>
+        <v>2400000</v>
       </c>
       <c r="E5" s="20">
-        <f>C5*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>223968.69705259849</v>
+        <f>C5*(WACC!$B$2*(1+WACC!$B$2)^$B5)/((1+WACC!$B$2)^$B5-1)</f>
+        <v>170285.89751815109</v>
       </c>
       <c r="F5" s="20">
-        <f>D5*(WACC!$B$1*(1+WACC!$B$1)^itm_invest!$B$2)/((1+WACC!$B$1)^itm_invest!$B$2-1)</f>
-        <v>153980.287397609</v>
-      </c>
+        <f>D5*(WACC!$C$2*(1+WACC!$C$2)^$B5)/((1+WACC!$C$2)^$B5-1)</f>
+        <v>153628.71068749097</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="23"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="21"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="21"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="7"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="21"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="21"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="21"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="21"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -11070,17 +11349,285 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E36C909-04D9-4788-9010-9C6CB2BA0080}">
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2" s="20">
+        <v>560000</v>
+      </c>
+      <c r="D2" s="20">
+        <v>560000</v>
+      </c>
+      <c r="E2" s="20">
+        <f>C2*(WACC!$B$2*(1+WACC!$B$2)^$B2)/((1+WACC!$B$2)^$B2-1)</f>
+        <v>39733.376087568584</v>
+      </c>
+      <c r="F2" s="20">
+        <f>D2*(WACC!$C$2*(1+WACC!$C$2)^$B2)/((1+WACC!$C$2)^$B2-1)</f>
+        <v>35846.699160414559</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3" s="20">
+        <v>3800000</v>
+      </c>
+      <c r="D3" s="20">
+        <v>3800000</v>
+      </c>
+      <c r="E3" s="20">
+        <f>C3*(WACC!$B$2*(1+WACC!$B$2)^$B3)/((1+WACC!$B$2)^$B3-1)</f>
+        <v>195022.11237084537</v>
+      </c>
+      <c r="F3" s="20">
+        <f>D3*(WACC!$C$2*(1+WACC!$C$2)^$B3)/((1+WACC!$C$2)^$B3-1)</f>
+        <v>160470.20579380851</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" s="20">
+        <v>1250000</v>
+      </c>
+      <c r="D4" s="20">
+        <v>1200000</v>
+      </c>
+      <c r="E4" s="20">
+        <f>C4*(WACC!$B$2*(1+WACC!$B$2)^$B4)/((1+WACC!$B$2)^$B4-1)</f>
+        <v>88690.571624037024</v>
+      </c>
+      <c r="F4" s="20">
+        <f>D4*(WACC!$C$2*(1+WACC!$C$2)^$B4)/((1+WACC!$C$2)^$B4-1)</f>
+        <v>76814.355343745483</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5" s="20">
+        <v>2400000</v>
+      </c>
+      <c r="D5" s="20">
+        <v>2400000</v>
+      </c>
+      <c r="E5" s="20">
+        <f>C5*(WACC!$B$2*(1+WACC!$B$2)^$B5)/((1+WACC!$B$2)^$B5-1)</f>
+        <v>170285.89751815109</v>
+      </c>
+      <c r="F5" s="20">
+        <f>D5*(WACC!$C$2*(1+WACC!$C$2)^$B5)/((1+WACC!$C$2)^$B5-1)</f>
+        <v>153628.71068749097</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8">
+        <v>925.309699999994</v>
+      </c>
+      <c r="D8" s="23">
+        <f>C2/C8</f>
+        <v>605.20277697294603</v>
+      </c>
+      <c r="E8" s="22">
+        <f>E2/C8</f>
+        <v>42.940624190548142</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="21">
+        <v>4962.8818000000101</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="22">
+        <f>E3/C9</f>
+        <v>39.296142892390662</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2101.9277999999999</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="22">
+        <f>E4/C10</f>
+        <v>42.194870644004531</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="7"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="21">
+        <v>874.98299999999904</v>
+      </c>
+      <c r="D12" s="7">
+        <f>D2/C12</f>
+        <v>640.01243452730012</v>
+      </c>
+      <c r="E12" s="22">
+        <f>F2/C12</f>
+        <v>40.968452141829722</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="21">
+        <v>3815.9558999999999</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="22">
+        <f t="shared" ref="E13:E15" si="0">F3/C13</f>
+        <v>42.052426704881078</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1513.7326</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="22">
+        <f t="shared" si="0"/>
+        <v>50.744996404084503</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="21">
+        <v>3255.9469999999801</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="22">
+        <f t="shared" si="0"/>
+        <v>47.184032997924078</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -11186,8 +11733,8 @@
         <v>6000000</v>
       </c>
       <c r="Q2" s="20">
-        <f>P2*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>259574.26734277737</v>
+        <f>P2*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>349668.96699620999</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -11240,8 +11787,8 @@
         <v>1500000</v>
       </c>
       <c r="Q3" s="20">
-        <f>P3*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>64893.566835694342</v>
+        <f>P3*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>87417.241749052497</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -11294,8 +11841,8 @@
         <v>1500000</v>
       </c>
       <c r="Q4" s="20">
-        <f>P4*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>64893.566835694342</v>
+        <f>P4*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>87417.241749052497</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -11348,8 +11895,8 @@
         <v>1750000</v>
       </c>
       <c r="Q5" s="20">
-        <f>P5*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>75709.161308310067</v>
+        <f>P5*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>101986.78204056126</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -11402,8 +11949,8 @@
         <v>1750000</v>
       </c>
       <c r="Q6" s="20">
-        <f>P6*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>75709.161308310067</v>
+        <f>P6*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>101986.78204056126</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -11456,8 +12003,8 @@
         <v>1500000</v>
       </c>
       <c r="Q7" s="20">
-        <f>P7*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>64893.566835694342</v>
+        <f>P7*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>87417.241749052497</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -11510,8 +12057,8 @@
         <v>1500000</v>
       </c>
       <c r="Q8" s="20">
-        <f>P8*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>64893.566835694342</v>
+        <f>P8*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>87417.241749052497</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -11564,8 +12111,8 @@
         <v>1600000</v>
       </c>
       <c r="Q9" s="20">
-        <f>P9*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>69219.804624740631</v>
+        <f>P9*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>93245.05786565601</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -11618,8 +12165,8 @@
         <v>1600000</v>
       </c>
       <c r="Q10" s="20">
-        <f>P10*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>69219.804624740631</v>
+        <f>P10*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>93245.05786565601</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -11672,8 +12219,8 @@
         <v>1750000</v>
       </c>
       <c r="Q11" s="20">
-        <f>P11*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>75709.161308310067</v>
+        <f>P11*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>101986.78204056126</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -11726,8 +12273,8 @@
         <v>1750000</v>
       </c>
       <c r="Q12" s="20">
-        <f>P12*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>75709.161308310067</v>
+        <f>P12*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>101986.78204056126</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -11780,8 +12327,8 @@
         <v>1800000</v>
       </c>
       <c r="Q13" s="20">
-        <f>P13*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>77872.280202833208</v>
+        <f>P13*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>104900.69009886299</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -11834,8 +12381,8 @@
         <v>525000</v>
       </c>
       <c r="Q14" s="20">
-        <f>P14*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>22712.74839249302</v>
+        <f>P14*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>30596.034612168376</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -11888,8 +12435,8 @@
         <v>525000</v>
       </c>
       <c r="Q15" s="20">
-        <f>P15*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>22712.74839249302</v>
+        <f>P15*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>30596.034612168376</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -11942,8 +12489,8 @@
         <v>550000</v>
       </c>
       <c r="Q16" s="20">
-        <f>P16*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>23794.307839754594</v>
+        <f>P16*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>32052.988641319247</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -11996,8 +12543,8 @@
         <v>550000</v>
       </c>
       <c r="Q17" s="20">
-        <f>P17*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>23794.307839754594</v>
+        <f>P17*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>32052.988641319247</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -12050,8 +12597,8 @@
         <v>575000</v>
       </c>
       <c r="Q18" s="20">
-        <f>P18*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>24875.867287016168</v>
+        <f>P18*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>33509.942670470125</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -12104,8 +12651,8 @@
         <v>575000</v>
       </c>
       <c r="Q19" s="20">
-        <f>P19*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>24875.867287016168</v>
+        <f>P19*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>33509.942670470125</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -12158,8 +12705,8 @@
         <v>700000</v>
       </c>
       <c r="Q20" s="20">
-        <f>P20*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>30283.664523324031</v>
+        <f>P20*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>40794.712816224499</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -12212,8 +12759,8 @@
         <v>700000</v>
       </c>
       <c r="Q21" s="20">
-        <f>P21*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>30283.664523324031</v>
+        <f>P21*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>40794.712816224499</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -12266,8 +12813,8 @@
         <v>800000</v>
       </c>
       <c r="Q22" s="20">
-        <f>P22*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>34609.902312370315</v>
+        <f>P22*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>46622.528932828005</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -12320,8 +12867,8 @@
         <v>800000</v>
       </c>
       <c r="Q23" s="20">
-        <f>P23*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>34609.902312370315</v>
+        <f>P23*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>46622.528932828005</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -12374,8 +12921,8 @@
         <v>800000</v>
       </c>
       <c r="Q24" s="20">
-        <f>P24*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>34609.902312370315</v>
+        <f>P24*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>46622.528932828005</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -12428,8 +12975,8 @@
         <v>800000</v>
       </c>
       <c r="Q25" s="20">
-        <f>P25*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>34609.902312370315</v>
+        <f>P25*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>46622.528932828005</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -12482,8 +13029,8 @@
         <v>200000</v>
       </c>
       <c r="Q26" s="20">
-        <f>P26*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>8652.4755780925789</v>
+        <f>P26*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>11655.632233207001</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -12536,8 +13083,8 @@
         <v>500000</v>
       </c>
       <c r="Q27" s="20">
-        <f>P27*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>21631.18894523145</v>
+        <f>P27*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>29139.080583017501</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -12590,8 +13137,8 @@
         <v>500000</v>
       </c>
       <c r="Q28" s="20">
-        <f>P28*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>21631.18894523145</v>
+        <f>P28*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>29139.080583017501</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -12644,8 +13191,8 @@
         <v>500000</v>
       </c>
       <c r="Q29" s="20">
-        <f>P29*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>21631.18894523145</v>
+        <f>P29*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>29139.080583017501</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -12698,8 +13245,8 @@
         <v>500000</v>
       </c>
       <c r="Q30" s="20">
-        <f>P30*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>21631.18894523145</v>
+        <f>P30*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>29139.080583017501</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -12752,8 +13299,8 @@
         <v>500000</v>
       </c>
       <c r="Q31" s="20">
-        <f>P31*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>21631.18894523145</v>
+        <f>P31*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>29139.080583017501</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -12806,8 +13353,8 @@
         <v>500000</v>
       </c>
       <c r="Q32" s="20">
-        <f>P32*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>21631.18894523145</v>
+        <f>P32*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>29139.080583017501</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -12860,8 +13407,8 @@
         <v>3000000</v>
       </c>
       <c r="Q33" s="20">
-        <f>P33*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>129787.13367138868</v>
+        <f>P33*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>174834.48349810499</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -12914,8 +13461,8 @@
         <v>2500000</v>
       </c>
       <c r="Q34" s="20">
-        <f>P34*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>108155.94472615725</v>
+        <f>P34*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>145695.4029150875</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -12968,8 +13515,8 @@
         <v>2500000</v>
       </c>
       <c r="Q35" s="20">
-        <f>P35*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>108155.94472615725</v>
+        <f>P35*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>145695.4029150875</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -13022,8 +13569,8 @@
         <v>2350000</v>
       </c>
       <c r="Q36" s="20">
-        <f>P36*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>101666.5880425878</v>
+        <f>P36*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>136953.67874018225</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -13076,8 +13623,62 @@
         <v>2350000</v>
       </c>
       <c r="Q37" s="20">
-        <f>P37*(WACC!$B$1*(1+WACC!$B$1)^$O$2)/((1+WACC!$B$1)^$O$2-1)</f>
-        <v>101666.5880425878</v>
+        <f>P37*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>136953.67874018225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1.01</v>
+      </c>
+      <c r="J38">
+        <v>1.02</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>2</v>
+      </c>
+      <c r="N38">
+        <v>50</v>
+      </c>
+      <c r="O38">
+        <v>25</v>
+      </c>
+      <c r="P38" s="20">
+        <v>550000</v>
+      </c>
+      <c r="Q38" s="20">
+        <f>P38*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
+        <v>32052.988641319247</v>
       </c>
     </row>
   </sheetData>
@@ -13087,12 +13688,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -13325,6 +13924,32 @@
         <v>5.4269999999999996</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2018</v>
+      </c>
+      <c r="B9">
+        <v>1.4</v>
+      </c>
+      <c r="D9">
+        <v>3.0449999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>45.277000000000001</v>
+      </c>
+      <c r="G9">
+        <v>4.5069999999999997</v>
+      </c>
+      <c r="H9">
+        <v>52.564999999999998</v>
+      </c>
+      <c r="I9">
+        <v>6.4169999999999998</v>
+      </c>
+    </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="20"/>
     </row>
@@ -13345,11 +13970,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13566,7 +14192,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13717,10 +14343,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15590,7 +16216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15886,11 +16512,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17014,6 +17640,14 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>100</v>
+      </c>
+      <c r="B40" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17022,10 +17656,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17941,6 +18577,26 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>100</v>
+      </c>
+      <c r="B40" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.25</v>
+      </c>
+      <c r="F40">
+        <v>0.25</v>
+      </c>
+    </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D41" s="7"/>
       <c r="E41" s="5"/>
@@ -17973,10 +18629,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18412,6 +19070,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>100</v>
+      </c>
+      <c r="B40" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>